<commit_message>
Edited pump pressure functions
</commit_message>
<xml_diff>
--- a/Interpolation fucntions.xlsx
+++ b/Interpolation fucntions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/pb745_cam_ac_uk/Documents/Studies/IIA/Projects/GA3 Heat exhanger/GA3-Heat-exchanger-optimisation-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{09920621-4704-4907-BD98-35197F71833D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA07A4E2-6ED7-45C7-AEA0-576AC0CB982B}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{09920621-4704-4907-BD98-35197F71833D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F9FEB77-5A9E-415E-86AF-C0FEABCE2B63}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9024" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
   </bookViews>
   <sheets>
     <sheet name="pump pressure drop and flowrate" sheetId="1" r:id="rId1"/>
@@ -999,6 +999,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>flow rate (litres/second)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1061,6 +1116,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>Pressure drop (bar)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2068,6 +2178,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>flow rate (litres/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2237,7 +2402,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15544564722088244"/>
+          <c:y val="0.16484444444444443"/>
+          <c:w val="0.79817937763216373"/>
+          <c:h val="0.52737672790901147"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -2294,8 +2469,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.30241644794400702"/>
-                  <c:y val="-0.14610199766695831"/>
+                  <c:x val="-0.3009624431233881"/>
+                  <c:y val="-8.3021790734939496E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2608,8 +2783,63 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>Sigma</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -2670,6 +2900,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>kc,ke</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5727,16 +6012,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>11429</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>59055</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6063,22 +6348,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E48BA44-5CBB-4482-B89C-29FF72610136}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6086,7 +6371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6094,7 +6379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.58330000000000004</v>
       </c>
@@ -6102,7 +6387,7 @@
         <v>0.1113</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.50829999999999997</v>
       </c>
@@ -6110,7 +6395,7 @@
         <v>0.2157</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.47499999999999998</v>
       </c>
@@ -6118,7 +6403,7 @@
         <v>0.25380000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.42499999999999999</v>
       </c>
@@ -6126,7 +6411,7 @@
         <v>0.31680000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.37919999999999998</v>
       </c>
@@ -6134,7 +6419,7 @@
         <v>0.36130000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.3417</v>
       </c>
@@ -6142,7 +6427,7 @@
         <v>0.40310000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.29580000000000001</v>
       </c>
@@ -6150,7 +6435,7 @@
         <v>0.4511</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.25829999999999997</v>
       </c>
@@ -6158,7 +6443,7 @@
         <v>0.48459999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.21249999999999999</v>
       </c>
@@ -6166,7 +6451,7 @@
         <v>0.5181</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.17080000000000001</v>
       </c>
@@ -6174,12 +6459,12 @@
         <v>0.55730000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -6187,7 +6472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -6195,7 +6480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.45829999999999999</v>
       </c>
@@ -6203,7 +6488,7 @@
         <v>0.1333</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.42359999999999998</v>
       </c>
@@ -6211,7 +6496,7 @@
         <v>0.17560000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.40100000000000002</v>
       </c>
@@ -6219,7 +6504,7 @@
         <v>0.2024</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.36109999999999998</v>
       </c>
@@ -6227,7 +6512,7 @@
         <v>0.25769999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.3125</v>
       </c>
@@ -6235,7 +6520,7 @@
         <v>0.31709999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.26390000000000002</v>
       </c>
@@ -6243,7 +6528,7 @@
         <v>0.36330000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.22220000000000001</v>
       </c>
@@ -6251,7 +6536,7 @@
         <v>0.42330000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.15970000000000001</v>
       </c>
@@ -6259,7 +6544,7 @@
         <v>0.47839999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.1181</v>
       </c>
@@ -6267,7 +6552,7 @@
         <v>0.53300000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6.9400000000000003E-2</v>
       </c>
@@ -6286,16 +6571,16 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -6306,7 +6591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -6317,7 +6602,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -6328,7 +6613,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -6339,7 +6624,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -6350,7 +6635,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -6361,7 +6646,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -6372,7 +6657,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -6383,7 +6668,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -6394,7 +6679,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -6405,7 +6690,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Created pitch shape function
</commit_message>
<xml_diff>
--- a/Interpolation fucntions.xlsx
+++ b/Interpolation fucntions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/pb745_cam_ac_uk/Documents/Studies/IIA/Projects/GA3 Heat exhanger/GA3-Heat-exchanger-optimisation-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{09920621-4704-4907-BD98-35197F71833D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F9FEB77-5A9E-415E-86AF-C0FEABCE2B63}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="8_{09920621-4704-4907-BD98-35197F71833D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0FA2256-0E93-4F99-A312-EFC238A8CB7A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
   </bookViews>
   <sheets>
     <sheet name="pump pressure drop and flowrate" sheetId="1" r:id="rId1"/>
@@ -1690,6 +1690,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>flow rate (litres/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5936,15 +5991,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>331470</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>26670</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6349,7 +6404,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Values to test in spreadsheet
</commit_message>
<xml_diff>
--- a/Interpolation fucntions.xlsx
+++ b/Interpolation fucntions.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/pb745_cam_ac_uk/Documents/Studies/IIA/Projects/GA3 Heat exhanger/GA3-Heat-exchanger-optimisation-code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Uni\IIA\Heat Exchanger\GA3-Heat-exchanger-optimisation-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="8_{09920621-4704-4907-BD98-35197F71833D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0FA2256-0E93-4F99-A312-EFC238A8CB7A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75FDAC4-6F8D-4A12-844E-B34C14B351FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
   </bookViews>
   <sheets>
     <sheet name="pump pressure drop and flowrate" sheetId="1" r:id="rId1"/>
     <sheet name="entrance exit pressure losses" sheetId="2" r:id="rId2"/>
+    <sheet name="Possible Geometries" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>COLD SIDE (2022)</t>
   </si>
@@ -64,12 +65,66 @@
   <si>
     <t>Kc turbulent</t>
   </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>square</t>
+  </si>
+  <si>
+    <t>nt</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>l_ends</t>
+  </si>
+  <si>
+    <t>lt_auto</t>
+  </si>
+  <si>
+    <t>lt_total</t>
+  </si>
+  <si>
+    <t>Flavour</t>
+  </si>
+  <si>
+    <t>odd</t>
+  </si>
+  <si>
+    <t>weird</t>
+  </si>
+  <si>
+    <t>sqaure</t>
+  </si>
+  <si>
+    <t>d_sh</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>n_cross</t>
+  </si>
+  <si>
+    <t>triangle</t>
+  </si>
+  <si>
+    <t>hexagon</t>
+  </si>
+  <si>
+    <t>star</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,13 +132,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,8 +166,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6403,22 +6475,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E48BA44-5CBB-4482-B89C-29FF72610136}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6426,7 +6498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6434,7 +6506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.58330000000000004</v>
       </c>
@@ -6442,7 +6514,7 @@
         <v>0.1113</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.50829999999999997</v>
       </c>
@@ -6450,7 +6522,7 @@
         <v>0.2157</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.47499999999999998</v>
       </c>
@@ -6458,7 +6530,7 @@
         <v>0.25380000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.42499999999999999</v>
       </c>
@@ -6466,7 +6538,7 @@
         <v>0.31680000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.37919999999999998</v>
       </c>
@@ -6474,7 +6546,7 @@
         <v>0.36130000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.3417</v>
       </c>
@@ -6482,7 +6554,7 @@
         <v>0.40310000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.29580000000000001</v>
       </c>
@@ -6490,7 +6562,7 @@
         <v>0.4511</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.25829999999999997</v>
       </c>
@@ -6498,7 +6570,7 @@
         <v>0.48459999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.21249999999999999</v>
       </c>
@@ -6506,7 +6578,7 @@
         <v>0.5181</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0.17080000000000001</v>
       </c>
@@ -6514,12 +6586,12 @@
         <v>0.55730000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -6527,7 +6599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -6535,7 +6607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0.45829999999999999</v>
       </c>
@@ -6543,7 +6615,7 @@
         <v>0.1333</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0.42359999999999998</v>
       </c>
@@ -6551,7 +6623,7 @@
         <v>0.17560000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0.40100000000000002</v>
       </c>
@@ -6559,7 +6631,7 @@
         <v>0.2024</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0.36109999999999998</v>
       </c>
@@ -6567,7 +6639,7 @@
         <v>0.25769999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0.3125</v>
       </c>
@@ -6575,7 +6647,7 @@
         <v>0.31709999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0.26390000000000002</v>
       </c>
@@ -6583,7 +6655,7 @@
         <v>0.36330000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0.22220000000000001</v>
       </c>
@@ -6591,7 +6663,7 @@
         <v>0.42330000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0.15970000000000001</v>
       </c>
@@ -6599,7 +6671,7 @@
         <v>0.47839999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0.1181</v>
       </c>
@@ -6607,7 +6679,7 @@
         <v>0.53300000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6.9400000000000003E-2</v>
       </c>
@@ -6629,13 +6701,13 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -6646,7 +6718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -6657,7 +6729,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -6668,7 +6740,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -6679,7 +6751,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -6690,7 +6762,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -6701,7 +6773,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -6712,7 +6784,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -6723,7 +6795,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -6734,7 +6806,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -6745,7 +6817,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -6760,4 +6832,417 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17164505-3E2F-4059-8633-DD8051065C5E}">
+  <dimension ref="B2:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <f>2*SQRT(2)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I3">
+        <v>3.5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <f>MIN(H3-(2*J3),(I3-G3*V3)/E3)</f>
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="L3" s="3">
+        <f>B3/(F3+1)</f>
+        <v>1.6717047997679452E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I4">
+        <v>3.5</v>
+      </c>
+      <c r="J4" s="1">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="K4" s="2">
+        <f>MIN(H4-(2*J4),(I4-G4*V4)/E4)</f>
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" ref="L4:L12" si="0">B4/(F4+1)</f>
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2">
+        <f>3*SQRT(2)</f>
+        <v>4.2426406871192857</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I5">
+        <v>3.5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="K5" s="2">
+        <f>MIN(H5-(2*J5),(I5-G5*V5)/E5)</f>
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2207588469154955E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2">
+        <f>SQRT(10)+1</f>
+        <v>4.16227766016838</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I6">
+        <v>3.5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <f>MIN(H6-(2*J6),(I6-G6*V6)/E6)</f>
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2397628375129378E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I7">
+        <v>3.5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <f>MIN(H7-(2*J7),(I7-G7*V7)/E7)</f>
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2">
+        <f>4*SQRT(2)</f>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.216</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I8">
+        <v>3.5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <f>MIN(H8-(2*J8),(I8-G8*V8)/E8)</f>
+        <v>0.21875</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="0"/>
+        <v>9.6141507086294296E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I9">
+        <v>3.5</v>
+      </c>
+      <c r="J9" s="1">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" ref="K9:K12" si="1">MIN(H9-(2*J9),(I9-G9*V9)/E9)</f>
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I10">
+        <v>3.5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="0"/>
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="2">
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <f>(2*SQRT(3))+1</f>
+        <v>4.4641016151377544</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I11">
+        <v>3.5</v>
+      </c>
+      <c r="J11" s="1">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1712812921102038E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="I12">
+        <v>3.5</v>
+      </c>
+      <c r="J12" s="1">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.21875</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0666666666666666E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Slightly improved hydraulic function iteration
</commit_message>
<xml_diff>
--- a/Interpolation fucntions.xlsx
+++ b/Interpolation fucntions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Uni\IIA\Heat Exchanger\GA3-Heat-exchanger-optimisation-code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/pb745_cam_ac_uk/Documents/Studies/IIA/Projects/GA3 Heat exhanger/GA3-Heat-exchanger-optimisation-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8612510-C937-4371-AF48-2AB404548DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
   </bookViews>
   <sheets>
     <sheet name="pump pressure drop and flowrate" sheetId="1" r:id="rId1"/>
@@ -6478,22 +6478,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E48BA44-5CBB-4482-B89C-29FF72610136}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6501,7 +6501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.58330000000000004</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>0.1113</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.50829999999999997</v>
       </c>
@@ -6525,7 +6525,7 @@
         <v>0.2157</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.47499999999999998</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>0.25380000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.42499999999999999</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>0.31680000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.37919999999999998</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>0.36130000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.3417</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>0.40310000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.29580000000000001</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>0.4511</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.25829999999999997</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>0.48459999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.21249999999999999</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>0.5181</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.17080000000000001</v>
       </c>
@@ -6589,12 +6589,12 @@
         <v>0.55730000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.45829999999999999</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>0.1333</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.42359999999999998</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>0.17560000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.40100000000000002</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>0.2024</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.36109999999999998</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>0.25769999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.3125</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>0.31709999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.26390000000000002</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>0.36330000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.22220000000000001</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>0.42330000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.15970000000000001</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>0.47839999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.1181</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>0.53300000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6.9400000000000003E-2</v>
       </c>
@@ -6704,13 +6704,13 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -6732,7 +6732,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -6743,7 +6743,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -6754,7 +6754,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -6798,7 +6798,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -6841,13 +6841,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17164505-3E2F-4059-8633-DD8051065C5E}">
   <dimension ref="B2:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>21</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>1.6717047997679452E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -6957,7 +6957,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -6995,7 +6995,7 @@
         <v>1.2207588469154955E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>1.2397628375129378E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>1.0666666666666666E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7108,7 +7108,7 @@
         <v>9.6141507086294296E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>2.1333333333333333E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7176,7 +7176,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7211,7 +7211,7 @@
         <v>1.1712812921102038E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>6.4000000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
Corrected hydraulic and thermal functions for multipass
</commit_message>
<xml_diff>
--- a/Interpolation fucntions.xlsx
+++ b/Interpolation fucntions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/pb745_cam_ac_uk/Documents/Studies/IIA/Projects/GA3 Heat exhanger/GA3-Heat-exchanger-optimisation-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8612510-C937-4371-AF48-2AB404548DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{B8612510-C937-4371-AF48-2AB404548DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E81B97D5-DBE2-4CE6-90E6-83514DAB0894}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
   </bookViews>
   <sheets>
     <sheet name="pump pressure drop and flowrate" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>COLD SIDE (2022)</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>triangular</t>
+  </si>
+  <si>
+    <t>JPL 2018</t>
+  </si>
+  <si>
+    <t>2017 B</t>
   </si>
 </sst>
 </file>
@@ -287,7 +293,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'pump pressure drop and flowrate'!$B$2:$B$3</c:f>
+              <c:f>'pump pressure drop and flowrate'!$C$2:$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -368,7 +374,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'pump pressure drop and flowrate'!$A$4:$A$13</c:f>
+              <c:f>'pump pressure drop and flowrate'!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -407,7 +413,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'pump pressure drop and flowrate'!$B$4:$B$13</c:f>
+              <c:f>'pump pressure drop and flowrate'!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -448,6 +454,124 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BFD3-4974-9AE7-A7DE5CBA0DDC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>JPL 2018</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pump pressure drop and flowrate'!$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.45400000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pump pressure drop and flowrate'!$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.27700000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9CB0-48FB-A7F9-C086D4C13E77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2017 B</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pump pressure drop and flowrate'!$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pump pressure drop and flowrate'!$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.47099999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9CB0-48FB-A7F9-C086D4C13E77}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -514,6 +638,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.36461260852008881"/>
+              <c:y val="0.80677990918790954"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -869,7 +1001,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'pump pressure drop and flowrate'!$B$16:$B$18</c:f>
+              <c:f>'pump pressure drop and flowrate'!$C$18:$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -959,7 +1091,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'pump pressure drop and flowrate'!$A$19:$A$28</c:f>
+              <c:f>'pump pressure drop and flowrate'!$B$21:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -998,7 +1130,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'pump pressure drop and flowrate'!$B$19:$B$28</c:f>
+              <c:f>'pump pressure drop and flowrate'!$C$21:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1039,6 +1171,124 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C3EB-411C-87E3-A6622E038A85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>JPL 2018</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pump pressure drop and flowrate'!$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.47199999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pump pressure drop and flowrate'!$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.13700000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9378-4B0B-A646-4C810E55F735}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2017 B</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pump pressure drop and flowrate'!$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.42499999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pump pressure drop and flowrate'!$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.21199999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9378-4B0B-A646-4C810E55F735}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1528,7 +1778,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'pump pressure drop and flowrate'!$B$4:$B$13</c:f>
+              <c:f>'pump pressure drop and flowrate'!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1567,7 +1817,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'pump pressure drop and flowrate'!$A$4:$A$13</c:f>
+              <c:f>'pump pressure drop and flowrate'!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2071,7 +2321,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'pump pressure drop and flowrate'!$B$19:$B$28</c:f>
+              <c:f>'pump pressure drop and flowrate'!$C$21:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2110,7 +2360,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'pump pressure drop and flowrate'!$A$19:$A$28</c:f>
+              <c:f>'pump pressure drop and flowrate'!$B$21:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5993,15 +6243,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>53340</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6029,16 +6279,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6065,16 +6315,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>331470</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>443865</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>26670</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>139065</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6101,16 +6351,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6476,218 +6726,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E48BA44-5CBB-4482-B89C-29FF72610136}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4">
         <v>0.58330000000000004</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.1113</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5">
         <v>0.50829999999999997</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.2157</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6">
         <v>0.47499999999999998</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.25380000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7">
         <v>0.42499999999999999</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.31680000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8">
         <v>0.37919999999999998</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.36130000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9">
         <v>0.3417</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>0.40310000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10">
         <v>0.29580000000000001</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>0.4511</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11">
         <v>0.25829999999999997</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>0.48459999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12">
         <v>0.21249999999999999</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0.5181</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>0.17080000000000001</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>0.55730000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="C14">
+        <v>0.27700000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>0.25</v>
+      </c>
+      <c r="C15">
+        <v>0.47099999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21">
         <v>0.45829999999999999</v>
       </c>
-      <c r="B19">
+      <c r="C21">
         <v>0.1333</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22">
         <v>0.42359999999999998</v>
       </c>
-      <c r="B20">
+      <c r="C22">
         <v>0.17560000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23">
         <v>0.40100000000000002</v>
       </c>
-      <c r="B21">
+      <c r="C23">
         <v>0.2024</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24">
         <v>0.36109999999999998</v>
       </c>
-      <c r="B22">
+      <c r="C24">
         <v>0.25769999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25">
         <v>0.3125</v>
       </c>
-      <c r="B23">
+      <c r="C25">
         <v>0.31709999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26">
         <v>0.26390000000000002</v>
       </c>
-      <c r="B24">
+      <c r="C26">
         <v>0.36330000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27">
         <v>0.22220000000000001</v>
       </c>
-      <c r="B25">
+      <c r="C27">
         <v>0.42330000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28">
         <v>0.15970000000000001</v>
       </c>
-      <c r="B26">
+      <c r="C28">
         <v>0.47839999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29">
         <v>0.1181</v>
       </c>
-      <c r="B27">
+      <c r="C29">
         <v>0.53300000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30">
         <v>6.9400000000000003E-2</v>
       </c>
-      <c r="B28">
+      <c r="C30">
         <v>0.57150000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="C31">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="C32">
+        <v>0.21199999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -6704,13 +6998,13 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -6721,7 +7015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -6732,7 +7026,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -6743,7 +7037,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -6754,7 +7048,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -6765,7 +7059,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -6776,7 +7070,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -6787,7 +7081,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -6798,7 +7092,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -6809,7 +7103,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -6820,7 +7114,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -6845,9 +7139,9 @@
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>21</v>
       </c>
@@ -6882,7 +7176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -6920,7 +7214,7 @@
         <v>1.6717047997679452E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -6957,7 +7251,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -6995,7 +7289,7 @@
         <v>1.2207588469154955E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7033,7 +7327,7 @@
         <v>1.2397628375129378E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7070,7 +7364,7 @@
         <v>1.0666666666666666E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7108,7 +7402,7 @@
         <v>9.6141507086294296E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7142,7 +7436,7 @@
         <v>2.1333333333333333E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7176,7 +7470,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7211,7 +7505,7 @@
         <v>1.1712812921102038E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>6.4000000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
Collect top n designs
</commit_message>
<xml_diff>
--- a/Interpolation fucntions.xlsx
+++ b/Interpolation fucntions.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{B8612510-C937-4371-AF48-2AB404548DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E81B97D5-DBE2-4CE6-90E6-83514DAB0894}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
   </bookViews>
   <sheets>
     <sheet name="pump pressure drop and flowrate" sheetId="1" r:id="rId1"/>
@@ -6728,22 +6728,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E48BA44-5CBB-4482-B89C-29FF72610136}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -6751,7 +6751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -6759,7 +6759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.58330000000000004</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>0.1113</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0.50829999999999997</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>0.2157</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0.47499999999999998</v>
       </c>
@@ -6783,7 +6783,7 @@
         <v>0.25380000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0.42499999999999999</v>
       </c>
@@ -6791,7 +6791,7 @@
         <v>0.31680000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.37919999999999998</v>
       </c>
@@ -6799,7 +6799,7 @@
         <v>0.36130000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.3417</v>
       </c>
@@ -6807,7 +6807,7 @@
         <v>0.40310000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.29580000000000001</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>0.4511</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.25829999999999997</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>0.48459999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0.21249999999999999</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>0.5181</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.17080000000000001</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>0.55730000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>0.27700000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -6861,12 +6861,12 @@
         <v>0.47099999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>0.45829999999999999</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>0.1333</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0.42359999999999998</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>0.17560000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>0.40100000000000002</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>0.2024</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>0.36109999999999998</v>
       </c>
@@ -6914,7 +6914,7 @@
         <v>0.25769999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>0.3125</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>0.31709999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>0.26390000000000002</v>
       </c>
@@ -6930,7 +6930,7 @@
         <v>0.36330000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>0.22220000000000001</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>0.42330000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>0.15970000000000001</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>0.47839999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0.1181</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>0.53300000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>6.9400000000000003E-2</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>0.57150000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -6994,17 +6994,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AF0AEE-4634-4177-A322-755E1ED26919}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -7037,7 +7037,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -7048,7 +7048,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -7059,7 +7059,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -7081,7 +7081,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -7092,7 +7092,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -7103,7 +7103,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -7139,9 +7139,9 @@
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>21</v>
       </c>
@@ -7176,7 +7176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>1.6717047997679452E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7251,7 +7251,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>1.2207588469154955E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7327,7 +7327,7 @@
         <v>1.2397628375129378E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7364,7 +7364,7 @@
         <v>1.0666666666666666E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7402,7 +7402,7 @@
         <v>9.6141507086294296E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7436,7 +7436,7 @@
         <v>2.1333333333333333E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7470,7 +7470,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -7505,7 +7505,7 @@
         <v>1.1712812921102038E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>6.4000000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
new file for different tube numbers
</commit_message>
<xml_diff>
--- a/Interpolation fucntions.xlsx
+++ b/Interpolation fucntions.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/pb745_cam_ac_uk/Documents/Studies/IIA/Projects/GA3 Heat exhanger/GA3-Heat-exchanger-optimisation-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{B8612510-C937-4371-AF48-2AB404548DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3E7587F-7ACF-417A-9F97-089123DF15A3}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="13_ncr:1_{B8612510-C937-4371-AF48-2AB404548DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B5A0D21-D405-4BE3-BE1D-09ACFC62D589}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CFDD6F95-EE7A-410D-8DA9-034F9A066FBE}"/>
   </bookViews>
   <sheets>
     <sheet name="pump pressure drop and flowrate" sheetId="1" r:id="rId1"/>
-    <sheet name="entrance exit pressure losses" sheetId="2" r:id="rId2"/>
-    <sheet name="Possible Geometries" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="entrance exit pressure losses" sheetId="2" r:id="rId3"/>
+    <sheet name="Possible Geometries" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>COLD SIDE (2022)</t>
   </si>
@@ -128,12 +129,115 @@
   <si>
     <t>2017 B</t>
   </si>
+  <si>
+    <t>JPL-2018 HX</t>
+  </si>
+  <si>
+    <t>LMTD</t>
+  </si>
+  <si>
+    <t>e-NTU</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Q (kW)</t>
+  </si>
+  <si>
+    <t>Effectiveness</t>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="6.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">hot  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(l/s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="6.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (l/s)</t>
+    </r>
+  </si>
+  <si>
+    <t>B-2017 HX</t>
+  </si>
+  <si>
+    <t>number tubes</t>
+  </si>
+  <si>
+    <t>number baffles</t>
+  </si>
+  <si>
+    <t>number of shell passes</t>
+  </si>
+  <si>
+    <t>number of tube passes</t>
+  </si>
+  <si>
+    <t>length of copper tubes</t>
+  </si>
+  <si>
+    <t>Pitch spacing</t>
+  </si>
+  <si>
+    <t>Number of shell rows crossed</t>
+  </si>
+  <si>
+    <t>Hydraulic analysis</t>
+  </si>
+  <si>
+    <t>Thermal analysis</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +248,29 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="6.6"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -163,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -171,16 +298,345 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3333,7 +3789,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'pump pressure drop and flowrate'!$B$32</c15:sqref>
@@ -3351,7 +3807,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'pump pressure drop and flowrate'!$C$32</c15:sqref>
@@ -3368,7 +3824,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-898D-491B-B1D2-3607EF1B7C96}"/>
                   </c:ext>
@@ -8329,7 +8785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E48BA44-5CBB-4482-B89C-29FF72610136}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
@@ -8592,6 +9048,174 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3E342A5-F6EF-4408-8144-DA7DDFD6D87A}">
+  <dimension ref="C1:O13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C8" s="17"/>
+      <c r="D8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="20"/>
+      <c r="L8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C9" s="21"/>
+      <c r="D9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C10" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.51</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="14">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="L10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="14">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="H11" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="L11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C12" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="15">
+        <v>15.622</v>
+      </c>
+      <c r="E12" s="6">
+        <v>15.622</v>
+      </c>
+      <c r="F12" s="16">
+        <v>14.79</v>
+      </c>
+      <c r="G12" s="10">
+        <v>10.33</v>
+      </c>
+      <c r="H12" s="16">
+        <v>13.01</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="24">
+        <v>0.1847</v>
+      </c>
+      <c r="E13" s="25">
+        <v>0.1847</v>
+      </c>
+      <c r="F13" s="26">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="G13" s="27">
+        <v>0.2152</v>
+      </c>
+      <c r="H13" s="26">
+        <v>0.314</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AF0AEE-4634-4177-A322-755E1ED26919}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -8732,7 +9356,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17164505-3E2F-4059-8633-DD8051065C5E}">
   <dimension ref="B2:L12"/>
   <sheetViews>

</xml_diff>